<commit_message>
updated week 8 hours
</commit_message>
<xml_diff>
--- a/personal-logs/Luka Vukovic.xlsx
+++ b/personal-logs/Luka Vukovic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luka\Documents\GitHub\Capstone-Project\personal-logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A03CF02-0318-466B-B069-C2B3C9C4994B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09293D8C-7DBC-4963-B32F-86AEED072A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11370" yWindow="3075" windowWidth="22695" windowHeight="15720" tabRatio="787" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11715" yWindow="3420" windowWidth="22695" windowHeight="15720" tabRatio="787" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="10" r:id="rId1"/>
@@ -983,784 +983,7 @@
     <cellStyle name="Total" xfId="41" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="42" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="541">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="430">
     <dxf>
       <fill>
         <patternFill>
@@ -5416,212 +4639,212 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A21">
-    <cfRule type="expression" dxfId="540" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="429" priority="50" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:B17">
-    <cfRule type="expression" dxfId="539" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="428" priority="22" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="expression" dxfId="538" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="427" priority="21" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="expression" dxfId="537" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="426" priority="20" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32:A36">
-    <cfRule type="expression" dxfId="536" priority="74" stopIfTrue="1">
+    <cfRule type="expression" dxfId="425" priority="74" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:A31">
-    <cfRule type="expression" dxfId="535" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="424" priority="41" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="expression" dxfId="532" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="423" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="expression" dxfId="531" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="422" priority="57" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17">
-    <cfRule type="expression" dxfId="530" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="421" priority="56" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="expression" dxfId="529" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="420" priority="55" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20">
-    <cfRule type="expression" dxfId="528" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="419" priority="51" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17">
-    <cfRule type="expression" dxfId="527" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="418" priority="60" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="expression" dxfId="526" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="417" priority="59" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:A15">
-    <cfRule type="expression" dxfId="525" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="416" priority="58" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20">
-    <cfRule type="expression" dxfId="524" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="415" priority="54" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18:A19">
-    <cfRule type="expression" dxfId="523" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="414" priority="53" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22">
-    <cfRule type="expression" dxfId="522" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="413" priority="52" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26">
-    <cfRule type="expression" dxfId="521" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="412" priority="49" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="expression" dxfId="520" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="411" priority="48" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A24">
-    <cfRule type="expression" dxfId="519" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="410" priority="47" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27">
-    <cfRule type="expression" dxfId="518" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="409" priority="46" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="expression" dxfId="517" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="408" priority="45" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26">
-    <cfRule type="expression" dxfId="516" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="407" priority="44" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="expression" dxfId="512" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="406" priority="36" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="expression" dxfId="511" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="405" priority="34" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="expression" dxfId="510" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="404" priority="19" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22:B26">
-    <cfRule type="expression" dxfId="509" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="403" priority="30" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="expression" dxfId="508" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="402" priority="17" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="expression" dxfId="507" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="401" priority="16" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="expression" dxfId="506" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="400" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="expression" dxfId="505" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="399" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="expression" dxfId="504" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="398" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="expression" dxfId="503" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="397" priority="23" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="expression" dxfId="502" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="396" priority="18" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26">
-    <cfRule type="expression" dxfId="501" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="395" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="expression" dxfId="500" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="394" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="expression" dxfId="499" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="393" priority="13" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32:B36">
-    <cfRule type="expression" dxfId="498" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="392" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="expression" dxfId="497" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="391" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28:B31">
-    <cfRule type="expression" dxfId="496" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="390" priority="6" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="expression" dxfId="495" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="389" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="expression" dxfId="494" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="388" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5908,277 +5131,277 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B27">
-    <cfRule type="expression" dxfId="491" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="387" priority="17" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="expression" dxfId="490" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="386" priority="16" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32:B33">
-    <cfRule type="expression" dxfId="489" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="385" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30">
-    <cfRule type="expression" dxfId="488" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="384" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37">
-    <cfRule type="expression" dxfId="484" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="383" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34">
-    <cfRule type="expression" dxfId="483" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="382" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35">
-    <cfRule type="expression" dxfId="482" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="381" priority="8" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34">
-    <cfRule type="expression" dxfId="481" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="380" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19">
-    <cfRule type="expression" dxfId="480" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="379" priority="48" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="expression" dxfId="477" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="378" priority="45" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:A22">
-    <cfRule type="expression" dxfId="476" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="377" priority="44" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="expression" dxfId="475" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="376" priority="43" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:B29">
-    <cfRule type="expression" dxfId="474" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="375" priority="31" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="expression" dxfId="473" priority="67" stopIfTrue="1">
+    <cfRule type="expression" dxfId="374" priority="67" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="expression" dxfId="471" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="373" priority="13" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="expression" dxfId="470" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="372" priority="42" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="expression" dxfId="469" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="371" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="expression" dxfId="468" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="370" priority="72" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="expression" dxfId="467" priority="90" stopIfTrue="1">
+    <cfRule type="expression" dxfId="369" priority="90" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30">
-    <cfRule type="expression" dxfId="466" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="368" priority="37" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28">
-    <cfRule type="expression" dxfId="465" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="367" priority="36" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24">
-    <cfRule type="expression" dxfId="463" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="366" priority="41" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="expression" dxfId="462" priority="92" stopIfTrue="1">
+    <cfRule type="expression" dxfId="365" priority="92" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:A15">
-    <cfRule type="expression" dxfId="461" priority="91" stopIfTrue="1">
+    <cfRule type="expression" dxfId="364" priority="91" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29">
-    <cfRule type="expression" dxfId="460" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="363" priority="35" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31">
-    <cfRule type="expression" dxfId="459" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="362" priority="34" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="expression" dxfId="457" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="361" priority="30" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="expression" dxfId="456" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="360" priority="29" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="expression" dxfId="455" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="359" priority="28" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="expression" dxfId="454" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="358" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="expression" dxfId="453" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="357" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:B20">
-    <cfRule type="expression" dxfId="452" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="356" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="expression" dxfId="451" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="355" priority="23" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="expression" dxfId="450" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="354" priority="22" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="expression" dxfId="448" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="353" priority="21" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="expression" dxfId="445" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="352" priority="71" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="expression" dxfId="444" priority="70" stopIfTrue="1">
+    <cfRule type="expression" dxfId="351" priority="70" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="expression" dxfId="438" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="350" priority="6" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="expression" dxfId="437" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="349" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="expression" dxfId="436" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="348" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="expression" dxfId="435" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="347" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="expression" dxfId="434" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="346" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="expression" dxfId="433" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="345" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32:A33">
-    <cfRule type="expression" dxfId="386" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="344" priority="52" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20">
-    <cfRule type="expression" dxfId="382" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="343" priority="47" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24">
-    <cfRule type="expression" dxfId="381" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="342" priority="46" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20">
-    <cfRule type="expression" dxfId="379" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="341" priority="51" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19">
-    <cfRule type="expression" dxfId="378" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="340" priority="50" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17:A18">
-    <cfRule type="expression" dxfId="377" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="339" priority="49" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29">
-    <cfRule type="expression" dxfId="373" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="338" priority="40" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28">
-    <cfRule type="expression" dxfId="372" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="337" priority="39" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:A27">
-    <cfRule type="expression" dxfId="371" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="336" priority="38" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="expression" dxfId="363" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="335" priority="20" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="expression" dxfId="362" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="334" priority="19" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="expression" dxfId="356" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="333" priority="18" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6208,21 +5431,21 @@
     <col min="4" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
     </row>
-    <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C3" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
@@ -6230,7 +5453,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -6238,32 +5461,32 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
     </row>
-    <row r="9" spans="1:3" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.3">
       <c r="A11" s="9"/>
       <c r="C11" s="10"/>
     </row>
-    <row r="12" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C12" s="10"/>
     </row>
-    <row r="13" spans="1:3" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>0</v>
       </c>
@@ -6272,7 +5495,7 @@
       </c>
       <c r="C13" s="12"/>
     </row>
-    <row r="14" spans="1:3" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
         <v>28</v>
       </c>
@@ -6280,7 +5503,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
         <v>29</v>
       </c>
@@ -6288,7 +5511,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>30</v>
       </c>
@@ -6296,7 +5519,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:2" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="45" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
         <v>31</v>
       </c>
@@ -6304,7 +5527,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
         <v>19</v>
       </c>
@@ -6312,7 +5535,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
         <v>33</v>
       </c>
@@ -6320,7 +5543,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
         <v>53</v>
       </c>
@@ -6328,79 +5551,79 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="13"/>
       <c r="B21" s="14"/>
     </row>
-    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="13"/>
       <c r="B22" s="14"/>
     </row>
-    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="13"/>
     </row>
-    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="14"/>
       <c r="B24" s="13"/>
     </row>
-    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="13"/>
       <c r="B25" s="13"/>
     </row>
-    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="13"/>
       <c r="B26" s="13"/>
     </row>
-    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="13"/>
       <c r="B27" s="14"/>
     </row>
-    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="14"/>
       <c r="B28" s="14"/>
     </row>
-    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
       <c r="B29" s="13"/>
     </row>
-    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
     </row>
-    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
     </row>
-    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
     </row>
-    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
     </row>
-    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="14"/>
       <c r="B34" s="13"/>
     </row>
-    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
     </row>
-    <row r="36" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
     </row>
-    <row r="37" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="13"/>
       <c r="B37" s="13"/>
     </row>
-    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="17"/>
       <c r="B38" s="18"/>
     </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="19" t="s">
         <v>6</v>
       </c>
@@ -6409,330 +5632,330 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A40" s="21"/>
       <c r="B40" s="22"/>
       <c r="C40" s="23"/>
     </row>
-    <row r="41" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="17" t="s">
         <v>7</v>
       </c>
       <c r="B41" s="24"/>
       <c r="C41" s="25"/>
     </row>
-    <row r="42" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="26"/>
       <c r="C42" s="27"/>
     </row>
-    <row r="43" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="26"/>
       <c r="C43" s="10"/>
     </row>
-    <row r="44" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="21"/>
       <c r="C44" s="10"/>
     </row>
-    <row r="45" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="28"/>
       <c r="C45" s="29"/>
     </row>
-    <row r="46" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C46" s="30"/>
     </row>
-    <row r="47" spans="1:3" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A47" s="31"/>
     </row>
-    <row r="49" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" s="32"/>
       <c r="C49" s="32"/>
     </row>
-    <row r="50" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50" s="33"/>
       <c r="C50" s="33"/>
     </row>
-    <row r="52" spans="2:3" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:3" ht="18" x14ac:dyDescent="0.35">
       <c r="B52" s="31"/>
       <c r="C52" s="31"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B16">
-    <cfRule type="expression" dxfId="338" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="332" priority="52" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="expression" dxfId="337" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="331" priority="55" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="expression" dxfId="336" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="330" priority="56" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="expression" dxfId="335" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="329" priority="58" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:A15">
-    <cfRule type="expression" dxfId="334" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="328" priority="57" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="expression" dxfId="333" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="327" priority="54" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="expression" dxfId="332" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="326" priority="53" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24">
-    <cfRule type="expression" dxfId="331" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="325" priority="40" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="expression" dxfId="330" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="324" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="expression" dxfId="329" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="323" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="expression" dxfId="328" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="322" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32:A33">
-    <cfRule type="expression" dxfId="327" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="321" priority="51" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31">
-    <cfRule type="expression" dxfId="326" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="320" priority="33" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="expression" dxfId="325" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="319" priority="31" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19">
-    <cfRule type="expression" dxfId="324" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="318" priority="47" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:A22">
-    <cfRule type="expression" dxfId="323" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="317" priority="43" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24">
-    <cfRule type="expression" dxfId="322" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="316" priority="45" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="expression" dxfId="321" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="315" priority="41" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19">
-    <cfRule type="expression" dxfId="319" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="314" priority="49" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17:A18">
-    <cfRule type="expression" dxfId="318" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="313" priority="48" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="expression" dxfId="317" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="312" priority="44" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="expression" dxfId="315" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="311" priority="42" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29">
-    <cfRule type="expression" dxfId="314" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="310" priority="39" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28">
-    <cfRule type="expression" dxfId="313" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="309" priority="38" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:A27">
-    <cfRule type="expression" dxfId="312" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="308" priority="37" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30">
-    <cfRule type="expression" dxfId="311" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="307" priority="36" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28">
-    <cfRule type="expression" dxfId="310" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="306" priority="35" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29">
-    <cfRule type="expression" dxfId="309" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="305" priority="34" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="expression" dxfId="308" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="304" priority="23" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:B29">
-    <cfRule type="expression" dxfId="307" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="303" priority="32" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="expression" dxfId="306" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="302" priority="21" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="expression" dxfId="305" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="301" priority="20" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="expression" dxfId="304" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="300" priority="30" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="expression" dxfId="303" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="299" priority="29" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="expression" dxfId="302" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="298" priority="28" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="expression" dxfId="301" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="297" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="expression" dxfId="300" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="296" priority="22" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="expression" dxfId="299" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="295" priority="19" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="expression" dxfId="298" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="294" priority="18" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="expression" dxfId="297" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="293" priority="17" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32:B33">
-    <cfRule type="expression" dxfId="296" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="292" priority="16" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30">
-    <cfRule type="expression" dxfId="295" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="291" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="expression" dxfId="294" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="290" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37">
-    <cfRule type="expression" dxfId="293" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="289" priority="13" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="expression" dxfId="292" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="288" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34">
-    <cfRule type="expression" dxfId="291" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="287" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35">
-    <cfRule type="expression" dxfId="290" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="286" priority="11" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34">
-    <cfRule type="expression" dxfId="289" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="285" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="expression" dxfId="288" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="284" priority="8" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="expression" dxfId="287" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="283" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="expression" dxfId="286" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="282" priority="6" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="expression" dxfId="285" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="281" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="expression" dxfId="284" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="280" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20">
-    <cfRule type="expression" dxfId="283" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="279" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="expression" dxfId="282" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="278" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="expression" dxfId="281" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="277" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6762,21 +5985,21 @@
     <col min="4" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
     </row>
-    <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C3" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
@@ -6784,7 +6007,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -6792,32 +6015,32 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
     </row>
-    <row r="9" spans="1:3" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.3">
       <c r="A11" s="9"/>
       <c r="C11" s="10"/>
     </row>
-    <row r="12" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C12" s="10"/>
     </row>
-    <row r="13" spans="1:3" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>0</v>
       </c>
@@ -6826,7 +6049,7 @@
       </c>
       <c r="C13" s="12"/>
     </row>
-    <row r="14" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
         <v>34</v>
       </c>
@@ -6834,7 +6057,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
         <v>32</v>
       </c>
@@ -6842,7 +6065,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>35</v>
       </c>
@@ -6850,7 +6073,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
         <v>36</v>
       </c>
@@ -6858,7 +6081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
         <v>37</v>
       </c>
@@ -6866,7 +6089,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:2" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
         <v>38</v>
       </c>
@@ -6874,7 +6097,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
         <v>39</v>
       </c>
@@ -6882,7 +6105,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
         <v>53</v>
       </c>
@@ -6890,7 +6113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="13" t="s">
         <v>60</v>
       </c>
@@ -6898,71 +6121,71 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="13"/>
     </row>
-    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="14"/>
       <c r="B24" s="13"/>
     </row>
-    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="13"/>
       <c r="B25" s="13"/>
     </row>
-    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="13"/>
       <c r="B26" s="13"/>
     </row>
-    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="13"/>
       <c r="B27" s="14"/>
     </row>
-    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="14"/>
       <c r="B28" s="14"/>
     </row>
-    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
       <c r="B29" s="13"/>
     </row>
-    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
     </row>
-    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
     </row>
-    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
     </row>
-    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
     </row>
-    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="14"/>
       <c r="B34" s="13"/>
     </row>
-    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
     </row>
-    <row r="36" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
     </row>
-    <row r="37" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="13"/>
       <c r="B37" s="13"/>
     </row>
-    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="17"/>
       <c r="B38" s="18"/>
     </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="19" t="s">
         <v>6</v>
       </c>
@@ -6971,332 +6194,332 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A40" s="21"/>
       <c r="B40" s="22"/>
       <c r="C40" s="23"/>
     </row>
-    <row r="41" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="17" t="s">
         <v>7</v>
       </c>
       <c r="B41" s="24"/>
       <c r="C41" s="25"/>
     </row>
-    <row r="42" spans="1:3" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A42" s="26" t="s">
         <v>61</v>
       </c>
       <c r="C42" s="27"/>
     </row>
-    <row r="43" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="26"/>
       <c r="C43" s="10"/>
     </row>
-    <row r="44" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="21"/>
       <c r="C44" s="10"/>
     </row>
-    <row r="45" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="28"/>
       <c r="C45" s="29"/>
     </row>
-    <row r="46" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C46" s="30"/>
     </row>
-    <row r="47" spans="1:3" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A47" s="31"/>
     </row>
-    <row r="49" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" s="32"/>
       <c r="C49" s="32"/>
     </row>
-    <row r="50" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50" s="33"/>
       <c r="C50" s="33"/>
     </row>
-    <row r="52" spans="2:3" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:3" ht="18" x14ac:dyDescent="0.35">
       <c r="B52" s="31"/>
       <c r="C52" s="31"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B16">
-    <cfRule type="expression" dxfId="280" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="276" priority="52" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="expression" dxfId="279" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="275" priority="55" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="expression" dxfId="278" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="274" priority="56" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="expression" dxfId="277" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="273" priority="58" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:A15">
-    <cfRule type="expression" dxfId="276" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="272" priority="57" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="expression" dxfId="275" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="271" priority="54" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="expression" dxfId="274" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="270" priority="53" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24">
-    <cfRule type="expression" dxfId="273" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="269" priority="40" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:B20">
-    <cfRule type="expression" dxfId="272" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="268" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="expression" dxfId="271" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="267" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="expression" dxfId="270" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="266" priority="21" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32:A33">
-    <cfRule type="expression" dxfId="269" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="265" priority="51" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31">
-    <cfRule type="expression" dxfId="268" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="264" priority="33" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="expression" dxfId="267" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="263" priority="31" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19">
-    <cfRule type="expression" dxfId="266" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="262" priority="47" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20">
-    <cfRule type="expression" dxfId="265" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="261" priority="46" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24">
-    <cfRule type="expression" dxfId="264" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="260" priority="45" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="expression" dxfId="263" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="259" priority="41" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20">
-    <cfRule type="expression" dxfId="262" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="258" priority="50" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19">
-    <cfRule type="expression" dxfId="261" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="257" priority="49" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17:A18">
-    <cfRule type="expression" dxfId="260" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="256" priority="48" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="expression" dxfId="259" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="255" priority="44" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22">
-    <cfRule type="expression" dxfId="258" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="254" priority="43" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="expression" dxfId="257" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="253" priority="42" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29">
-    <cfRule type="expression" dxfId="256" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="252" priority="39" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28">
-    <cfRule type="expression" dxfId="255" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="251" priority="38" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:A27">
-    <cfRule type="expression" dxfId="254" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="250" priority="37" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30">
-    <cfRule type="expression" dxfId="253" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="249" priority="36" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28">
-    <cfRule type="expression" dxfId="252" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="248" priority="35" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29">
-    <cfRule type="expression" dxfId="251" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="247" priority="34" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="expression" dxfId="250" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="246" priority="23" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:B29">
-    <cfRule type="expression" dxfId="249" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="245" priority="32" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="expression" dxfId="247" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="244" priority="20" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="expression" dxfId="246" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="243" priority="30" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="expression" dxfId="245" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="242" priority="29" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="expression" dxfId="244" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="241" priority="28" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="expression" dxfId="242" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="240" priority="22" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="expression" dxfId="241" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="239" priority="19" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="expression" dxfId="240" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="238" priority="18" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="expression" dxfId="239" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="237" priority="17" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32:B33">
-    <cfRule type="expression" dxfId="238" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="236" priority="16" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30">
-    <cfRule type="expression" dxfId="237" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="235" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="expression" dxfId="236" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="234" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37">
-    <cfRule type="expression" dxfId="235" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="233" priority="13" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="expression" dxfId="234" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="232" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34">
-    <cfRule type="expression" dxfId="233" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="231" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35">
-    <cfRule type="expression" dxfId="232" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="230" priority="11" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34">
-    <cfRule type="expression" dxfId="231" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="229" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="expression" dxfId="230" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="228" priority="8" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="expression" dxfId="229" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="227" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="expression" dxfId="228" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="226" priority="6" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="expression" dxfId="227" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="225" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="expression" dxfId="226" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="224" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="expression" dxfId="225" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="223" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="expression" dxfId="224" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="222" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="expression" dxfId="223" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="221" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7326,21 +6549,21 @@
     <col min="4" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
     </row>
-    <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C3" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
@@ -7348,7 +6571,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -7356,32 +6579,32 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
     </row>
-    <row r="9" spans="1:3" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.3">
       <c r="A11" s="9"/>
       <c r="C11" s="10"/>
     </row>
-    <row r="12" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C12" s="10"/>
     </row>
-    <row r="13" spans="1:3" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>0</v>
       </c>
@@ -7390,7 +6613,7 @@
       </c>
       <c r="C13" s="12"/>
     </row>
-    <row r="14" spans="1:3" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
         <v>40</v>
       </c>
@@ -7398,7 +6621,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
         <v>42</v>
       </c>
@@ -7406,7 +6629,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>43</v>
       </c>
@@ -7414,7 +6637,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:2" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
         <v>44</v>
       </c>
@@ -7422,7 +6645,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
         <v>46</v>
       </c>
@@ -7430,7 +6653,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
         <v>54</v>
       </c>
@@ -7438,83 +6661,83 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="13"/>
     </row>
-    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="13"/>
       <c r="B21" s="14"/>
     </row>
-    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="13"/>
       <c r="B22" s="14"/>
     </row>
-    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="13"/>
     </row>
-    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="14"/>
       <c r="B24" s="13"/>
     </row>
-    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="13"/>
       <c r="B25" s="13"/>
     </row>
-    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="13"/>
       <c r="B26" s="13"/>
     </row>
-    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="13"/>
       <c r="B27" s="14"/>
     </row>
-    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="14"/>
       <c r="B28" s="14"/>
     </row>
-    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
       <c r="B29" s="13"/>
     </row>
-    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
     </row>
-    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
     </row>
-    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
     </row>
-    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
     </row>
-    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="14"/>
       <c r="B34" s="13"/>
     </row>
-    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
     </row>
-    <row r="36" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
     </row>
-    <row r="37" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="13"/>
       <c r="B37" s="13"/>
     </row>
-    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="17"/>
       <c r="B38" s="18"/>
     </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="19" t="s">
         <v>6</v>
       </c>
@@ -7523,154 +6746,154 @@
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A40" s="21"/>
       <c r="B40" s="22"/>
       <c r="C40" s="23"/>
     </row>
-    <row r="41" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="17" t="s">
         <v>7</v>
       </c>
       <c r="B41" s="24"/>
       <c r="C41" s="25"/>
     </row>
-    <row r="42" spans="1:3" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A42" s="26" t="s">
         <v>41</v>
       </c>
       <c r="C42" s="27"/>
     </row>
-    <row r="43" spans="1:3" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="75" x14ac:dyDescent="0.3">
       <c r="A43" s="26" t="s">
         <v>45</v>
       </c>
       <c r="C43" s="10"/>
     </row>
-    <row r="44" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="21"/>
       <c r="C44" s="10"/>
     </row>
-    <row r="45" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="28"/>
       <c r="C45" s="29"/>
     </row>
-    <row r="46" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C46" s="30"/>
     </row>
-    <row r="47" spans="1:3" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A47" s="31"/>
     </row>
-    <row r="49" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" s="32"/>
       <c r="C49" s="32"/>
     </row>
-    <row r="50" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50" s="33"/>
       <c r="C50" s="33"/>
     </row>
-    <row r="52" spans="2:3" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:3" ht="18" x14ac:dyDescent="0.35">
       <c r="B52" s="31"/>
       <c r="C52" s="31"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B16">
-    <cfRule type="expression" dxfId="222" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="220" priority="52" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="expression" dxfId="221" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="219" priority="55" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="expression" dxfId="220" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="218" priority="56" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="expression" dxfId="219" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="217" priority="58" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:A15">
-    <cfRule type="expression" dxfId="218" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="216" priority="57" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="expression" dxfId="217" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="215" priority="54" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="expression" dxfId="216" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="214" priority="53" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24">
-    <cfRule type="expression" dxfId="215" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="213" priority="40" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="expression" dxfId="214" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="212" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="expression" dxfId="213" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="211" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="expression" dxfId="212" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="210" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32:A33">
-    <cfRule type="expression" dxfId="211" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="209" priority="51" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31">
-    <cfRule type="expression" dxfId="210" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="208" priority="33" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="expression" dxfId="209" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="207" priority="31" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="expression" dxfId="208" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="206" priority="44" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20">
-    <cfRule type="expression" dxfId="207" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="205" priority="46" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24">
-    <cfRule type="expression" dxfId="206" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="204" priority="45" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="expression" dxfId="205" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="203" priority="41" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20">
-    <cfRule type="expression" dxfId="204" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="202" priority="50" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17:A18">
-    <cfRule type="expression" dxfId="202" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="201" priority="48" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7880,21 +7103,21 @@
     <col min="4" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
     </row>
-    <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C3" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
@@ -7902,7 +7125,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -7910,32 +7133,32 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
     </row>
-    <row r="9" spans="1:3" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.3">
       <c r="A11" s="9"/>
       <c r="C11" s="10"/>
     </row>
-    <row r="12" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C12" s="10"/>
     </row>
-    <row r="13" spans="1:3" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>0</v>
       </c>
@@ -7944,7 +7167,7 @@
       </c>
       <c r="C13" s="12"/>
     </row>
-    <row r="14" spans="1:3" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
         <v>48</v>
       </c>
@@ -7952,7 +7175,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
         <v>49</v>
       </c>
@@ -7960,7 +7183,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>51</v>
       </c>
@@ -7968,7 +7191,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:2" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
         <v>50</v>
       </c>
@@ -7976,7 +7199,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
         <v>52</v>
       </c>
@@ -7984,7 +7207,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
         <v>19</v>
       </c>
@@ -7992,7 +7215,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
         <v>53</v>
       </c>
@@ -8000,79 +7223,79 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="13"/>
       <c r="B21" s="14"/>
     </row>
-    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="13"/>
       <c r="B22" s="14"/>
     </row>
-    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="13"/>
     </row>
-    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="14"/>
       <c r="B24" s="13"/>
     </row>
-    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="13"/>
       <c r="B25" s="13"/>
     </row>
-    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="13"/>
       <c r="B26" s="13"/>
     </row>
-    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="13"/>
       <c r="B27" s="14"/>
     </row>
-    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="14"/>
       <c r="B28" s="14"/>
     </row>
-    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
       <c r="B29" s="13"/>
     </row>
-    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
     </row>
-    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
     </row>
-    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
     </row>
-    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
     </row>
-    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="14"/>
       <c r="B34" s="13"/>
     </row>
-    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
     </row>
-    <row r="36" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
     </row>
-    <row r="37" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="13"/>
       <c r="B37" s="13"/>
     </row>
-    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="17"/>
       <c r="B38" s="18"/>
     </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="19" t="s">
         <v>6</v>
       </c>
@@ -8081,49 +7304,49 @@
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A40" s="21"/>
       <c r="B40" s="22"/>
       <c r="C40" s="23"/>
     </row>
-    <row r="41" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="17" t="s">
         <v>7</v>
       </c>
       <c r="B41" s="24"/>
       <c r="C41" s="25"/>
     </row>
-    <row r="42" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="26"/>
       <c r="C42" s="27"/>
     </row>
-    <row r="43" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="26"/>
       <c r="C43" s="10"/>
     </row>
-    <row r="44" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="21"/>
       <c r="C44" s="10"/>
     </row>
-    <row r="45" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="28"/>
       <c r="C45" s="29"/>
     </row>
-    <row r="46" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C46" s="30"/>
     </row>
-    <row r="47" spans="1:3" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A47" s="31"/>
     </row>
-    <row r="49" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" s="32"/>
       <c r="C49" s="32"/>
     </row>
-    <row r="50" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50" s="33"/>
       <c r="C50" s="33"/>
     </row>
-    <row r="52" spans="2:3" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:3" ht="18" x14ac:dyDescent="0.35">
       <c r="B52" s="31"/>
       <c r="C52" s="31"/>
     </row>
@@ -8990,8 +8213,8 @@
   </sheetPr>
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -9087,7 +8310,7 @@
         <v>73</v>
       </c>
       <c r="B16" s="13">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -9103,7 +8326,7 @@
         <v>75</v>
       </c>
       <c r="B18" s="13">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.3">
@@ -9111,7 +8334,7 @@
         <v>76</v>
       </c>
       <c r="B19" s="13">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -9196,7 +8419,7 @@
       </c>
       <c r="B39" s="20">
         <f>SUM(B14:B37)</f>
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.3">

</xml_diff>